<commit_message>
Locators Update for the framework
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/TestData.xlsx
+++ b/target/test-classes/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0320AE-DFE0-46BC-94AA-5B9B2AEB2B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C571BC5-44AD-4DFB-A9DC-4B5F77FA8A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
@@ -478,15 +478,15 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -500,7 +500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -514,7 +514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -537,27 +537,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D071FE2-89C5-4C36-B925-609C062F8AEB}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -598,7 +598,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -642,5 +642,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test data sheet
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/TestData.xlsx
+++ b/target/test-classes/testdata/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C571BC5-44AD-4DFB-A9DC-4B5F77FA8A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612CE102-E858-478B-B176-EE127386FBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="690" windowWidth="20490" windowHeight="10770" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
     <sheet name="CATSLogin" sheetId="12" r:id="rId2"/>
+    <sheet name="AgentLogin" sheetId="13" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>don1thack</t>
   </si>
@@ -65,9 +66,6 @@
     <t>CustomerNum</t>
   </si>
   <si>
-    <t>53357214</t>
-  </si>
-  <si>
     <t>SendLettersbyMail</t>
   </si>
   <si>
@@ -89,18 +87,12 @@
     <t>No</t>
   </si>
   <si>
-    <t>011000015</t>
-  </si>
-  <si>
     <t>BankAccountNum</t>
   </si>
   <si>
     <t>ReenterBankAccountNum</t>
   </si>
   <si>
-    <t>12345</t>
-  </si>
-  <si>
     <t>BankAccountType</t>
   </si>
   <si>
@@ -116,7 +108,13 @@
     <t>CalendarDay</t>
   </si>
   <si>
-    <t>13</t>
+    <t>HEALTHBENEFI</t>
+  </si>
+  <si>
+    <t>LetterName</t>
+  </si>
+  <si>
+    <t>Ptest</t>
   </si>
 </sst>
 </file>
@@ -181,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -190,6 +188,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -537,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D071FE2-89C5-4C36-B925-609C062F8AEB}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,34 +569,34 @@
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -605,38 +606,38 @@
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
+      <c r="C2" s="6">
+        <v>53357214</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="H2" s="6">
+        <v>11000015</v>
+      </c>
+      <c r="I2" s="6">
+        <v>12345</v>
+      </c>
+      <c r="J2" s="6">
+        <v>12345</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="M2" s="6">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -644,4 +645,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A6EE5C-BA51-4480-B29C-8CA8A4F57F00}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>